<commit_message>
Update sprint requirement stacks
</commit_message>
<xml_diff>
--- a/Documentation/Initial/Requirements/Requirements Stack.xlsx
+++ b/Documentation/Initial/Requirements/Requirements Stack.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StardewModding\EECS-581-Group-7-Project-3\Documentation\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StardewModding\EECS-581-Group-7-Project-3\Documentation\Initial\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B01CE14-E21A-47AF-9A8A-A3312DEF71C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BDF2AC9-8D71-40D6-B43B-64E2DDEFA51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -418,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -474,6 +474,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -812,7 +818,7 @@
   <dimension ref="A1:O91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,7 +859,9 @@
       <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="22" t="s">
+        <v>50</v>
+      </c>
       <c r="H2" s="10" t="s">
         <v>57</v>
       </c>
@@ -878,6 +886,9 @@
       <c r="D3" s="9" t="s">
         <v>61</v>
       </c>
+      <c r="E3" s="23">
+        <v>1</v>
+      </c>
       <c r="H3" s="13" t="s">
         <v>51</v>
       </c>
@@ -903,6 +914,9 @@
       </c>
       <c r="D4" s="6">
         <v>2</v>
+      </c>
+      <c r="E4" s="23">
+        <v>1</v>
       </c>
       <c r="H4" s="13"/>
       <c r="I4" s="14"/>
@@ -926,6 +940,9 @@
       <c r="D5" s="6">
         <v>3</v>
       </c>
+      <c r="E5" s="23">
+        <v>1</v>
+      </c>
       <c r="H5" s="16" t="s">
         <v>59</v>
       </c>
@@ -952,6 +969,7 @@
       <c r="D6" s="6">
         <v>4</v>
       </c>
+      <c r="E6" s="23"/>
       <c r="H6" s="17"/>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
@@ -974,7 +992,9 @@
       <c r="D7" s="7">
         <v>5</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -989,7 +1009,9 @@
       <c r="D8" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -1004,7 +1026,9 @@
       <c r="D9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1019,7 +1043,9 @@
       <c r="D10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="22" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1034,6 +1060,7 @@
       <c r="D11" s="6">
         <v>6</v>
       </c>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -1048,6 +1075,7 @@
       <c r="D12" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1062,6 +1090,7 @@
       <c r="D13" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="E13" s="23"/>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1076,7 +1105,7 @@
       <c r="D14" s="7">
         <v>7</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="22"/>
     </row>
     <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -1091,7 +1120,7 @@
       <c r="D15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1106,6 +1135,7 @@
       <c r="D16" s="6">
         <v>8</v>
       </c>
+      <c r="E16" s="23"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -1120,7 +1150,7 @@
       <c r="D17" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="22"/>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1135,7 +1165,7 @@
       <c r="D18" s="7">
         <v>9</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="22"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -1150,7 +1180,7 @@
       <c r="D19" s="7">
         <v>10</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1165,7 +1195,7 @@
       <c r="D20" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="22"/>
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1180,7 +1210,7 @@
       <c r="D21" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -1195,7 +1225,7 @@
       <c r="D22" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -1210,7 +1240,7 @@
       <c r="D23" s="7">
         <v>11</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1225,7 +1255,7 @@
       <c r="D24" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="22"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -1240,7 +1270,7 @@
       <c r="D25" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="22"/>
     </row>
     <row r="26" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -1255,7 +1285,7 @@
       <c r="D26" s="7">
         <v>12</v>
       </c>
-      <c r="E26" s="3"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -1270,7 +1300,7 @@
       <c r="D27" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -1285,7 +1315,7 @@
       <c r="D28" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="22"/>
     </row>
     <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -1300,6 +1330,7 @@
       <c r="D29" s="6">
         <v>13</v>
       </c>
+      <c r="E29" s="23"/>
     </row>
     <row r="30" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -1314,6 +1345,7 @@
       <c r="D30" s="6">
         <v>14</v>
       </c>
+      <c r="E30" s="23"/>
     </row>
     <row r="31" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -1328,6 +1360,7 @@
       <c r="D31" s="6">
         <v>15</v>
       </c>
+      <c r="E31" s="23"/>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
@@ -1342,6 +1375,7 @@
       <c r="D32" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="E32" s="23"/>
     </row>
     <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -1356,6 +1390,7 @@
       <c r="D33" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="E33" s="23"/>
     </row>
     <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
@@ -1370,6 +1405,7 @@
       <c r="D34" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="E34" s="23"/>
     </row>
     <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
@@ -1384,7 +1420,7 @@
       <c r="D35" s="7">
         <v>16</v>
       </c>
-      <c r="E35" s="3"/>
+      <c r="E35" s="22"/>
     </row>
     <row r="36" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
@@ -1399,7 +1435,7 @@
       <c r="D36" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="3"/>
+      <c r="E36" s="22"/>
     </row>
     <row r="37" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -1414,7 +1450,7 @@
       <c r="D37" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E37" s="3"/>
+      <c r="E37" s="22"/>
     </row>
     <row r="38" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
@@ -1429,7 +1465,7 @@
       <c r="D38" s="6">
         <v>17</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="23"/>
     </row>
     <row r="39" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
@@ -1444,6 +1480,7 @@
       <c r="D39" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="E39" s="23"/>
     </row>
     <row r="40" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
@@ -1458,6 +1495,7 @@
       <c r="D40" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="E40" s="23"/>
     </row>
     <row r="41" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
@@ -1472,6 +1510,7 @@
       <c r="D41" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
@@ -1486,6 +1525,7 @@
       <c r="D42" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="E42" s="23"/>
     </row>
     <row r="43" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -1500,7 +1540,7 @@
       <c r="D43" s="7">
         <v>18</v>
       </c>
-      <c r="E43" s="3"/>
+      <c r="E43" s="22"/>
     </row>
     <row r="44" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
@@ -1515,7 +1555,7 @@
       <c r="D44" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E44" s="3"/>
+      <c r="E44" s="22"/>
     </row>
     <row r="45" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
@@ -1530,7 +1570,7 @@
       <c r="D45" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E45" s="3"/>
+      <c r="E45" s="22"/>
     </row>
     <row r="46" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>

</xml_diff>

<commit_message>
Add completed stories documents for each sprint
</commit_message>
<xml_diff>
--- a/Documentation/Initial/Requirements/Requirements Stack.xlsx
+++ b/Documentation/Initial/Requirements/Requirements Stack.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\StardewModding\EECS-581-Group-7-Project-3\Documentation\Initial\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CAE33FB-8537-4FE3-BE37-73E6D54C745E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC05864-5C71-484B-8855-30C3E6E125B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Stack" sheetId="2" r:id="rId1"/>
@@ -817,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BF7F4D-835C-4109-BF21-40DBBF02C95A}">
   <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,7 +1318,7 @@
         <v>12</v>
       </c>
       <c r="E26" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1335,7 +1335,7 @@
         <v>51</v>
       </c>
       <c r="E27" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1352,7 +1352,7 @@
         <v>51</v>
       </c>
       <c r="E28" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1386,7 +1386,7 @@
         <v>14</v>
       </c>
       <c r="E30" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1403,7 +1403,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
         <v>51</v>
       </c>
       <c r="E32" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1437,7 +1437,7 @@
         <v>51</v>
       </c>
       <c r="E33" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1454,7 +1454,7 @@
         <v>51</v>
       </c>
       <c r="E34" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>